<commit_message>
"Return after being sick :("
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\PROJECTS\Excel Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B7AE13-88E7-4ACE-B064-1CD027F57AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827EA636-052D-40B0-B610-E5A6659547E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{D1FC2354-1431-294E-9D05-A71CF1B59C9B}"/>
   </bookViews>
@@ -21,6 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Raw!$E$3:$E$259</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Raw!$H$3:$H$259</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1044,6 +1045,9 @@
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.1</cx:f>
+      </cx:strDim>
       <cx:numDim type="val">
         <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
@@ -11247,7 +11251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DF77E48-6FD4-8644-A782-E6B1D9E27C39}">
   <dimension ref="B1:Q259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G18" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>

</xml_diff>